<commit_message>
added successful line of thrust on center of base method
</commit_message>
<xml_diff>
--- a/docs/input_template_lface2.xlsx
+++ b/docs/input_template_lface2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4189A3B-284A-1A41-A346-C1F0DAF8FE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FA3F5E-A386-9440-BEF8-D84F8011E991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20600" yWindow="860" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="35060" yWindow="1040" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1898,10 +1898,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>145.30000000000001</c:v>
+                  <c:v>115.69999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>170</c:v>
+                  <c:v>145.30000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1913,10 +1913,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>84</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4624,7 +4624,7 @@
   <dimension ref="A2:N36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B5"/>
+      <selection activeCell="D4" sqref="D4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5142,16 +5142,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5162,7 +5162,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5598,7 +5598,7 @@
   <dimension ref="A2:E20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5771,7 +5771,7 @@
   <dimension ref="A2:N18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6123,7 +6123,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C5"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6200,10 +6200,10 @@
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
-        <v>145.30000000000001</v>
+        <v>115.69999999999999</v>
       </c>
       <c r="C4" s="3">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3">
         <v>3000</v>
@@ -6220,10 +6220,10 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
-        <v>170</v>
+        <v>145.30000000000001</v>
       </c>
       <c r="C5" s="3">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3">
         <v>3000</v>

</xml_diff>

<commit_message>
fixed variable names in line_of_thrust_center function
</commit_message>
<xml_diff>
--- a/docs/input_template_lface2.xlsx
+++ b/docs/input_template_lface2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FA3F5E-A386-9440-BEF8-D84F8011E991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A46436-620F-6C45-8A38-7B02E45D09AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35060" yWindow="1040" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="36820" yWindow="740" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1897,12 +1897,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>115.69999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>145.30000000000001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1912,12 +1906,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6123,7 +6111,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="B4" sqref="B4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6199,15 +6187,9 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B4" s="3">
-        <v>115.69999999999999</v>
-      </c>
-      <c r="C4" s="3">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3000</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6219,15 +6201,9 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="3">
-        <v>145.30000000000001</v>
-      </c>
-      <c r="C5" s="3">
-        <v>64</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3000</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>

</xml_diff>

<commit_message>
archive point - working on spencer's method
</commit_message>
<xml_diff>
--- a/docs/input_template_lface2.xlsx
+++ b/docs/input_template_lface2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A46436-620F-6C45-8A38-7B02E45D09AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4333B3-3771-7440-BCB9-6CCC24D1E97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36820" yWindow="740" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="19360" yWindow="1580" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1897,6 +1897,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>145.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1906,6 +1912,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4612,7 +4624,7 @@
   <dimension ref="A2:N36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E5"/>
+      <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5130,16 +5142,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="M20:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6111,7 +6123,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D5"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6187,9 +6199,15 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="3">
+        <v>145.30000000000001</v>
+      </c>
+      <c r="C4" s="3">
+        <v>64</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1000</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6201,9 +6219,15 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" s="3">
+        <v>170</v>
+      </c>
+      <c r="C5" s="3">
+        <v>84</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1000</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>

</xml_diff>

<commit_message>
new spencer's method based on utexas2 user manual equations
</commit_message>
<xml_diff>
--- a/docs/input_template_lface2.xlsx
+++ b/docs/input_template_lface2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4333B3-3771-7440-BCB9-6CCC24D1E97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA5CACC-837D-204E-99BF-A6B12A65B86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19360" yWindow="1580" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="38780" yWindow="1900" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="126">
   <si>
     <t>X</t>
   </si>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>Distributed load set (b) is only used for rapid drawdown analysis</t>
+  </si>
+  <si>
+    <t>dl_top</t>
   </si>
 </sst>
 </file>
@@ -6120,10 +6123,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7976BB56-7732-404C-B58A-55DA7F8052B3}">
-  <dimension ref="B2:P29"/>
+  <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6558,6 +6561,39 @@
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="30" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>125</v>
+      </c>
+      <c r="G33">
+        <f>SQRT((B4-B5)^2 + (C4-C5)^2)</f>
+        <v>31.781913095344017</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <f>G33*D4</f>
+        <v>31781.913095344018</v>
+      </c>
+      <c r="K34">
+        <f>G34/2</f>
+        <v>15890.956547672009</v>
+      </c>
+      <c r="L34">
+        <f>K34*0.63</f>
+        <v>10011.302625033366</v>
+      </c>
+    </row>
+    <row r="37" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <f>12.35/0.777</f>
+        <v>15.894465894465894</v>
+      </c>
+      <c r="J37">
+        <f>15890.957*0.629</f>
+        <v>9995.4119530000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made spencer's solver more robust
</commit_message>
<xml_diff>
--- a/docs/input_template_lface2.xlsx
+++ b/docs/input_template_lface2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA5CACC-837D-204E-99BF-A6B12A65B86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D684B09-F14E-0344-8B9F-83D25096932C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38780" yWindow="1900" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
@@ -6126,7 +6126,7 @@
   <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6209,7 +6209,7 @@
         <v>64</v>
       </c>
       <c r="D4" s="3">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -6229,7 +6229,7 @@
         <v>84</v>
       </c>
       <c r="D5" s="3">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -6575,15 +6575,15 @@
     <row r="34" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G34">
         <f>G33*D4</f>
-        <v>31781.913095344018</v>
+        <v>63563.826190688036</v>
       </c>
       <c r="K34">
         <f>G34/2</f>
-        <v>15890.956547672009</v>
+        <v>31781.913095344018</v>
       </c>
       <c r="L34">
         <f>K34*0.63</f>
-        <v>10011.302625033366</v>
+        <v>20022.605250066732</v>
       </c>
     </row>
     <row r="37" spans="6:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added note to spencer.md on utexas2 equation source
</commit_message>
<xml_diff>
--- a/docs/input_template_lface2.xlsx
+++ b/docs/input_template_lface2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D684B09-F14E-0344-8B9F-83D25096932C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E7BE6C-A8C2-2B48-9731-47928AB3CDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38780" yWindow="1900" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="17560" yWindow="2000" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Improved solver efficiency for spencer's method. Checked FS_diff for various theta values before using the Newton solver. Also updated solution method in spencer.md.
</commit_message>
<xml_diff>
--- a/docs/input_template_lface2.xlsx
+++ b/docs/input_template_lface2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/CursorProjects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E7BE6C-A8C2-2B48-9731-47928AB3CDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DF934D-0569-BE45-966B-8A2F972AF8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17560" yWindow="2000" windowWidth="30020" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
@@ -1901,10 +1901,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>145.30000000000001</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>170</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1916,7 +1916,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>84</c:v>
@@ -4627,7 +4627,7 @@
   <dimension ref="A2:N36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B5"/>
+      <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5145,16 +5145,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6126,7 +6126,7 @@
   <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6203,10 +6203,10 @@
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
-        <v>145.30000000000001</v>
+        <v>170</v>
       </c>
       <c r="C4" s="3">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="D4" s="3">
         <v>2000</v>
@@ -6223,7 +6223,7 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="C5" s="3">
         <v>84</v>
@@ -6569,21 +6569,21 @@
       </c>
       <c r="G33">
         <f>SQRT((B4-B5)^2 + (C4-C5)^2)</f>
-        <v>31.781913095344017</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G34">
         <f>G33*D4</f>
-        <v>63563.826190688036</v>
+        <v>60000</v>
       </c>
       <c r="K34">
         <f>G34/2</f>
-        <v>31781.913095344018</v>
+        <v>30000</v>
       </c>
       <c r="L34">
         <f>K34*0.63</f>
-        <v>20022.605250066732</v>
+        <v>18900</v>
       </c>
     </row>
     <row r="37" spans="6:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
created a faster generate_slices funciton
</commit_message>
<xml_diff>
--- a/docs/input_template_lface2.xlsx
+++ b/docs/input_template_lface2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/CursorProjects/slopetools/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC635B6-EE88-8F4D-89C8-DC7541DFAC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB3F621-ED7F-9F4D-8AA6-A79F13A98B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17560" yWindow="2000" windowWidth="30020" windowHeight="24340" activeTab="1" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="36340" yWindow="1940" windowWidth="30020" windowHeight="24340" activeTab="5" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="126">
   <si>
     <t>X</t>
   </si>
@@ -1900,12 +1900,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1915,12 +1909,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>84</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4672,7 +4660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CEDAD3-D805-AE4D-9F0D-9E80BF51FF21}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -4688,7 +4676,7 @@
   <dimension ref="A2:N36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B6"/>
+      <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5834,8 +5822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE6F868-4227-8740-A8A1-4745562882FC}">
   <dimension ref="A2:N18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5893,7 +5881,7 @@
         <v>145</v>
       </c>
       <c r="C5" s="3">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>29</v>
@@ -5915,10 +5903,18 @@
       <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="3">
+        <v>145</v>
+      </c>
+      <c r="C6" s="3">
+        <v>120</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3">
+        <v>40</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -6187,7 +6183,7 @@
   <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6263,15 +6259,9 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B4" s="3">
-        <v>170</v>
-      </c>
-      <c r="C4" s="3">
-        <v>84</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2000</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6283,15 +6273,9 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="3">
-        <v>200</v>
-      </c>
-      <c r="C5" s="3">
-        <v>84</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2000</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6630,21 +6614,21 @@
       </c>
       <c r="G33">
         <f>SQRT((B4-B5)^2 + (C4-C5)^2)</f>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G34">
         <f>G33*D4</f>
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="K34">
         <f>G34/2</f>
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="L34">
         <f>K34*0.63</f>
-        <v>18900</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="6:12" x14ac:dyDescent="0.2">

</xml_diff>